<commit_message>
added accuracy and reproducibility segments to lab report
</commit_message>
<xml_diff>
--- a/Lab9/Accuracy.xlsx
+++ b/Lab9/Accuracy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel\Documents\EE445L\Lab9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D564ED7-7CAB-4431-801E-CE855CD1FD92}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AF4134-7B60-4357-B4ED-CB3760B4FD09}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{ABEB69AD-7D96-4E01-B2C6-EDC4D6465BBB}"/>
   </bookViews>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -441,14 +441,14 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>22.01</v>
+        <v>33.01</v>
       </c>
       <c r="C2">
-        <v>2200</v>
+        <v>3300</v>
       </c>
       <c r="D2">
         <f>C2/100</f>
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -456,14 +456,14 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C3">
-        <v>2203</v>
+        <v>3303</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D6" si="0">C3/100</f>
-        <v>22.03</v>
+        <v>33.03</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -471,14 +471,14 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>22.03</v>
+        <v>33.03</v>
       </c>
       <c r="C4">
-        <v>2200</v>
+        <v>3300</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -486,14 +486,14 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>21.98</v>
+        <v>32.979999999999997</v>
       </c>
       <c r="C5">
-        <v>2199</v>
+        <v>3299</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>21.99</v>
+        <v>32.99</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -501,20 +501,20 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C6">
-        <v>2193</v>
+        <v>3293</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>21.93</v>
+        <v>32.93</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D9">
         <f>ABS(B2-D2)</f>
-        <v>1.0000000000001563E-2</v>
+        <v>9.9999999999980105E-3</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -532,7 +532,7 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>9.9999999999980105E-3</v>
+        <v>1.0000000000005116E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -541,7 +541,7 @@
       </c>
       <c r="D13">
         <f>SUM(D9:D12)</f>
-        <v>8.0000000000001847E-2</v>
+        <v>8.00000000000054E-2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -550,7 +550,7 @@
       </c>
       <c r="D15">
         <f>D13/5</f>
-        <v>1.6000000000000368E-2</v>
+        <v>1.6000000000001079E-2</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.35">
@@ -559,7 +559,7 @@
       </c>
       <c r="D17" s="1">
         <f>D15</f>
-        <v>1.6000000000000368E-2</v>
+        <v>1.6000000000001079E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>